<commit_message>
Add example Data objects
</commit_message>
<xml_diff>
--- a/build_tools/Class_definitions/Class_definitions.xlsx
+++ b/build_tools/Class_definitions/Class_definitions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="293">
   <si>
     <t>Slot</t>
   </si>
@@ -898,6 +898,15 @@
   </si>
   <si>
     <t>Is Area 1 currently closed (TRUE) or open (FALSE)? Defaults to FALSE</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscellaneous list for bio-economic parameters </t>
   </si>
 </sst>
 </file>
@@ -1837,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2172,6 +2181,17 @@
       </c>
       <c r="D20" s="3" t="s">
         <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix index conditioning issue
</commit_message>
<xml_diff>
--- a/build_tools/Class_definitions/Class_definitions.xlsx
+++ b/build_tools/Class_definitions/Class_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\GitHub\MSEtool\build_tools\Class_definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38680FB7-6AC0-4C3B-93B8-36A03682A123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3709A00F-179C-4365-8776-232F7D90AAAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2385" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="614">
   <si>
     <t>Slot</t>
   </si>
@@ -1855,6 +1855,24 @@
   </si>
   <si>
     <t xml:space="preserve">Parameter controlling hyperstability/hyperdepletion where values below 1 lead to hyperstability (an index that decreases slower than true abundance) and values above 1 lead to hyperdepletion (an index that decreases more rapidly than true abundance). </t>
+  </si>
+  <si>
+    <t>I_beta</t>
+  </si>
+  <si>
+    <t>VI_beta</t>
+  </si>
+  <si>
+    <t>SpI_beta</t>
+  </si>
+  <si>
+    <t>Beta for hyperstability/depletion for `Data@Ind`</t>
+  </si>
+  <si>
+    <t>Beta for hyperstability/depletion for `Data@VInd`</t>
+  </si>
+  <si>
+    <t>Beta for hyperstability/depletion for `Data@SpInd`</t>
   </si>
 </sst>
 </file>
@@ -2804,7 +2822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -3168,7 +3186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>119</v>
       </c>
@@ -3188,7 +3206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>276</v>
       </c>
@@ -3233,7 +3251,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3891,10 +3909,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4927,57 +4945,57 @@
         <v>185</v>
       </c>
     </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>608</v>
+      </c>
+      <c r="B76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" t="s">
+        <v>611</v>
+      </c>
+      <c r="D76" t="s">
+        <v>185</v>
+      </c>
+    </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>216</v>
+        <v>609</v>
       </c>
       <c r="B77" t="s">
         <v>21</v>
       </c>
       <c r="C77" t="s">
-        <v>218</v>
+        <v>612</v>
       </c>
       <c r="D77" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>610</v>
       </c>
       <c r="B78" t="s">
         <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>220</v>
+        <v>613</v>
       </c>
       <c r="D78" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>221</v>
-      </c>
-      <c r="B79" t="s">
-        <v>21</v>
-      </c>
-      <c r="C79" t="s">
-        <v>222</v>
-      </c>
-      <c r="D79" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B80" t="s">
         <v>21</v>
       </c>
       <c r="C80" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D80" t="s">
         <v>217</v>
@@ -4985,13 +5003,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B81" t="s">
         <v>21</v>
       </c>
       <c r="C81" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D81" t="s">
         <v>217</v>
@@ -4999,29 +5017,71 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B82" t="s">
         <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D82" t="s">
         <v>217</v>
       </c>
     </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>223</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" t="s">
+        <v>224</v>
+      </c>
+      <c r="D83" t="s">
+        <v>217</v>
+      </c>
+    </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>225</v>
+      </c>
+      <c r="B84" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84" t="s">
+        <v>226</v>
+      </c>
+      <c r="D84" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>227</v>
+      </c>
+      <c r="B85" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D85" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>213</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B87" t="s">
         <v>214</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C87" t="s">
         <v>215</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D87" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update documentation for SPR
</commit_message>
<xml_diff>
--- a/build_tools/Class_definitions/Class_definitions.xlsx
+++ b/build_tools/Class_definitions/Class_definitions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2390" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-2390" windowWidth="29040" windowHeight="15840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
@@ -869,9 +869,6 @@
     <t>Observation parameters (last historical year used for time-varying parameters). Data.frame with `nsim` rows</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently not used. </t>
-  </si>
-  <si>
     <t>Named list with bio-economic output Only used if bio-economic parameters are included in OM</t>
   </si>
   <si>
@@ -1923,6 +1920,9 @@
   </si>
   <si>
     <t>Catch-at-age effective sample size. If greater than 1, then this is the multinomial distribution sample size. If less than 1, this is the coefficient of variation for the logistic normal distribution (see help doucmentation for simCAA for details).</t>
+  </si>
+  <si>
+    <t>Named list with equilibrium and dynamic SPR. Each element is an array with dimensions: nsim, nMPs, proyears. Non-negative real numbers.</t>
   </si>
 </sst>
 </file>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>0</v>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
@@ -2373,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
@@ -2394,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" t="s">
@@ -2415,7 +2415,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" t="s">
@@ -2436,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" t="s">
@@ -2457,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" t="s">
@@ -2478,7 +2478,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" t="s">
@@ -2499,7 +2499,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" t="s">
@@ -2520,7 +2520,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" t="s">
@@ -2541,7 +2541,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" t="s">
@@ -2562,7 +2562,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" t="s">
@@ -2583,7 +2583,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" t="s">
@@ -2604,7 +2604,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" t="s">
@@ -2625,7 +2625,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" t="s">
@@ -2646,7 +2646,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" t="s">
@@ -2667,7 +2667,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" t="s">
@@ -2688,7 +2688,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" t="s">
@@ -2709,7 +2709,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" t="s">
@@ -2730,7 +2730,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>0</v>
@@ -2751,7 +2751,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>0</v>
@@ -2772,7 +2772,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" t="s">
@@ -2793,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" t="s">
@@ -2814,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" t="s">
@@ -2835,7 +2835,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" t="s">
@@ -2921,7 +2921,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>0</v>
@@ -2941,7 +2941,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
@@ -2961,7 +2961,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
@@ -2978,7 +2978,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
@@ -2995,7 +2995,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>0</v>
@@ -3012,7 +3012,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
@@ -3032,7 +3032,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>200</v>
@@ -3052,10 +3052,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>16</v>
@@ -3072,10 +3072,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>16</v>
@@ -3092,10 +3092,10 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
@@ -3112,10 +3112,10 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>16</v>
@@ -3132,10 +3132,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>16</v>
@@ -3152,7 +3152,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E14" s="3" t="b">
         <v>0</v>
@@ -3169,10 +3169,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>16</v>
@@ -3189,10 +3189,10 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
@@ -3209,10 +3209,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>16</v>
@@ -3229,10 +3229,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>16</v>
@@ -3249,10 +3249,10 @@
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>16</v>
@@ -3269,13 +3269,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -3302,7 +3302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -3345,7 +3345,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -3359,7 +3359,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -3373,7 +3373,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -3387,10 +3387,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>16</v>
@@ -3404,10 +3404,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="F6" t="s">
         <v>629</v>
-      </c>
-      <c r="F6" t="s">
-        <v>630</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
@@ -3421,10 +3421,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
@@ -3438,10 +3438,10 @@
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
@@ -3455,7 +3455,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -3469,7 +3469,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -3483,7 +3483,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -3497,10 +3497,10 @@
         <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>16</v>
@@ -3514,7 +3514,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -3528,7 +3528,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -3542,7 +3542,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -3556,7 +3556,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -3570,7 +3570,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -3584,7 +3584,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -3598,7 +3598,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -3612,7 +3612,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -3626,7 +3626,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -3640,7 +3640,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -3654,7 +3654,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -3668,7 +3668,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -3682,7 +3682,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -3696,7 +3696,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -3710,7 +3710,7 @@
         <v>15</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -3724,7 +3724,7 @@
         <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -3732,13 +3732,13 @@
     </row>
     <row r="29" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -3746,13 +3746,13 @@
     </row>
     <row r="30" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -3760,13 +3760,13 @@
     </row>
     <row r="31" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -3828,7 +3828,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -3845,10 +3845,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>16</v>
@@ -3865,10 +3865,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
@@ -3885,10 +3885,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>16</v>
@@ -3905,10 +3905,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
@@ -3925,10 +3925,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
@@ -3945,10 +3945,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F8" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
@@ -3977,7 +3977,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -3991,13 +3991,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>441</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>442</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>80</v>
@@ -4008,7 +4008,7 @@
         <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
@@ -4089,13 +4089,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B9" t="s">
         <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D9" t="s">
         <v>80</v>
@@ -4106,7 +4106,7 @@
         <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C10" t="s">
         <v>118</v>
@@ -4120,7 +4120,7 @@
         <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C11" t="s">
         <v>114</v>
@@ -4176,7 +4176,7 @@
         <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C15" t="s">
         <v>116</v>
@@ -4190,7 +4190,7 @@
         <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C16" t="s">
         <v>112</v>
@@ -4201,13 +4201,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>446</v>
+      </c>
+      <c r="B17" t="s">
         <v>447</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>448</v>
-      </c>
-      <c r="C17" t="s">
-        <v>449</v>
       </c>
       <c r="D17" t="s">
         <v>80</v>
@@ -4215,13 +4215,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>449</v>
+      </c>
+      <c r="B18" t="s">
+        <v>447</v>
+      </c>
+      <c r="C18" t="s">
         <v>450</v>
-      </c>
-      <c r="B18" t="s">
-        <v>448</v>
-      </c>
-      <c r="C18" t="s">
-        <v>451</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
@@ -4232,7 +4232,7 @@
         <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C19" t="s">
         <v>110</v>
@@ -4243,13 +4243,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>451</v>
+      </c>
+      <c r="B20" t="s">
+        <v>447</v>
+      </c>
+      <c r="C20" t="s">
         <v>452</v>
-      </c>
-      <c r="B20" t="s">
-        <v>448</v>
-      </c>
-      <c r="C20" t="s">
-        <v>453</v>
       </c>
       <c r="D20" t="s">
         <v>80</v>
@@ -4260,7 +4260,7 @@
         <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C21" t="s">
         <v>120</v>
@@ -4355,13 +4355,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B28" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D28" t="s">
         <v>80</v>
@@ -4369,13 +4369,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B29" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C29" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D29" t="s">
         <v>80</v>
@@ -4383,13 +4383,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>625</v>
+      </c>
+      <c r="B30" t="s">
+        <v>445</v>
+      </c>
+      <c r="C30" t="s">
         <v>626</v>
-      </c>
-      <c r="B30" t="s">
-        <v>446</v>
-      </c>
-      <c r="C30" t="s">
-        <v>627</v>
       </c>
       <c r="D30" t="s">
         <v>80</v>
@@ -4439,13 +4439,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>454</v>
+      </c>
+      <c r="B36" t="s">
         <v>455</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>456</v>
-      </c>
-      <c r="C36" t="s">
-        <v>457</v>
       </c>
       <c r="D36" t="s">
         <v>127</v>
@@ -4456,7 +4456,7 @@
         <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C37" t="s">
         <v>133</v>
@@ -4484,7 +4484,7 @@
         <v>137</v>
       </c>
       <c r="B39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C39" t="s">
         <v>138</v>
@@ -4523,13 +4523,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>457</v>
+      </c>
+      <c r="B42" t="s">
         <v>458</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>459</v>
-      </c>
-      <c r="C42" t="s">
-        <v>460</v>
       </c>
       <c r="D42" t="s">
         <v>127</v>
@@ -4537,13 +4537,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>460</v>
+      </c>
+      <c r="B43" t="s">
         <v>461</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>462</v>
-      </c>
-      <c r="C43" t="s">
-        <v>463</v>
       </c>
       <c r="D43" t="s">
         <v>127</v>
@@ -4554,10 +4554,10 @@
         <v>233</v>
       </c>
       <c r="B44" t="s">
+        <v>463</v>
+      </c>
+      <c r="C44" t="s">
         <v>464</v>
-      </c>
-      <c r="C44" t="s">
-        <v>465</v>
       </c>
       <c r="D44" t="s">
         <v>127</v>
@@ -4565,13 +4565,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>465</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
         <v>466</v>
-      </c>
-      <c r="B46" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" t="s">
-        <v>467</v>
       </c>
       <c r="D46" t="s">
         <v>142</v>
@@ -4579,13 +4579,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>467</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
         <v>468</v>
-      </c>
-      <c r="B47" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" t="s">
-        <v>469</v>
       </c>
       <c r="D47" t="s">
         <v>142</v>
@@ -4593,13 +4593,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>469</v>
+      </c>
+      <c r="B48" t="s">
         <v>470</v>
       </c>
-      <c r="B48" t="s">
-        <v>471</v>
-      </c>
       <c r="C48" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D48" t="s">
         <v>142</v>
@@ -4607,13 +4607,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>610</v>
+      </c>
+      <c r="B49" t="s">
+        <v>470</v>
+      </c>
+      <c r="C49" t="s">
         <v>611</v>
-      </c>
-      <c r="B49" t="s">
-        <v>471</v>
-      </c>
-      <c r="C49" t="s">
-        <v>612</v>
       </c>
       <c r="D49" t="s">
         <v>142</v>
@@ -4621,13 +4621,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>471</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
         <v>472</v>
-      </c>
-      <c r="B50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" t="s">
-        <v>473</v>
       </c>
       <c r="D50" t="s">
         <v>142</v>
@@ -4635,13 +4635,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B51" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C51" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D51" t="s">
         <v>142</v>
@@ -4649,13 +4649,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B52" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C52" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D52" t="s">
         <v>142</v>
@@ -4663,13 +4663,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B53" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C53" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D53" t="s">
         <v>142</v>
@@ -4677,13 +4677,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B54" t="s">
         <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D54" t="s">
         <v>142</v>
@@ -4705,13 +4705,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B56" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C56" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D56" t="s">
         <v>142</v>
@@ -4789,13 +4789,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B62" t="s">
         <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D62" t="s">
         <v>142</v>
@@ -4803,13 +4803,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B63" t="s">
         <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D63" t="s">
         <v>142</v>
@@ -4817,13 +4817,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B64" t="s">
         <v>16</v>
       </c>
       <c r="C64" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D64" t="s">
         <v>142</v>
@@ -4831,13 +4831,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B65" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C65" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D65" t="s">
         <v>142</v>
@@ -4929,13 +4929,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B72" t="s">
         <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D72" t="s">
         <v>142</v>
@@ -4943,13 +4943,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B73" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C73" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D73" t="s">
         <v>142</v>
@@ -4957,13 +4957,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B74" t="s">
         <v>16</v>
       </c>
       <c r="C74" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D74" t="s">
         <v>142</v>
@@ -4971,13 +4971,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B75" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C75" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D75" t="s">
         <v>142</v>
@@ -4985,13 +4985,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B76" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C76" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D76" t="s">
         <v>142</v>
@@ -5055,13 +5055,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B81" t="s">
         <v>16</v>
       </c>
       <c r="C81" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D81" t="s">
         <v>142</v>
@@ -5069,13 +5069,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B82" t="s">
         <v>16</v>
       </c>
       <c r="C82" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D82" t="s">
         <v>142</v>
@@ -5083,13 +5083,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B83" t="s">
         <v>16</v>
       </c>
       <c r="C83" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D83" t="s">
         <v>142</v>
@@ -5097,44 +5097,44 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B85" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C85" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D85" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B86" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C86" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D86" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B87" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C87" t="s">
+        <v>618</v>
+      </c>
+      <c r="D87" t="s">
         <v>619</v>
-      </c>
-      <c r="D87" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
@@ -5245,8 +5245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5387,12 +5387,12 @@
         <v>276</v>
       </c>
       <c r="B17" t="s">
-        <v>279</v>
+        <v>630</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B18" t="s">
         <v>275</v>
@@ -5435,7 +5435,7 @@
         <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -5443,31 +5443,31 @@
         <v>263</v>
       </c>
       <c r="B24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B27" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -5475,7 +5475,7 @@
         <v>244</v>
       </c>
       <c r="B28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -5522,10 +5522,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -5541,7 +5541,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -5563,10 +5563,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -5574,26 +5574,26 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -5601,31 +5601,31 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -5633,95 +5633,95 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B24" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -5729,31 +5729,31 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B27" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -5766,10 +5766,10 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -5782,7 +5782,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
@@ -5790,28 +5790,28 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B38" t="s">
         <v>69</v>
@@ -5819,15 +5819,15 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B39" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B40" t="s">
         <v>70</v>
@@ -5835,15 +5835,15 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B43" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -5851,10 +5851,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -5862,10 +5862,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B45" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -5884,10 +5884,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B47" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -5895,10 +5895,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -5906,10 +5906,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -5917,10 +5917,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B50" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -5928,10 +5928,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B51" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -5939,10 +5939,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B52" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -5950,10 +5950,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B53" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -5966,7 +5966,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -5974,7 +5974,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -5982,7 +5982,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -5990,7 +5990,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -5998,7 +5998,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -6014,10 +6014,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B61" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -6030,10 +6030,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B63" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -6041,10 +6041,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B64" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -6052,10 +6052,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B65" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -6063,10 +6063,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B66" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -6074,10 +6074,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B67" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -6085,15 +6085,15 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B70" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -6101,10 +6101,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B71" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -6112,15 +6112,15 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B74" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -6139,10 +6139,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B76" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
@@ -6150,10 +6150,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B77" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
@@ -6161,191 +6161,191 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B80" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B81" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B82" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B83" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B84" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B85" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B86" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B87" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B88" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B89" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B90" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B91" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B92" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B93" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B94" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B95" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B96" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B97" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B98" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B99" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B100" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B101" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B102" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C102" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
add defaults to OM
and test for completeness

fixes #56
fixes #55
</commit_message>
<xml_diff>
--- a/build_tools/Class_definitions/Class_definitions.xlsx
+++ b/build_tools/Class_definitions/Class_definitions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2390" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="28680" yWindow="-2390" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="644">
   <si>
     <t>Slot</t>
   </si>
@@ -1929,6 +1929,39 @@
   </si>
   <si>
     <t>Natural mortality (M) by simulation, age and year. No variability is added</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Beverton-Holt</t>
+  </si>
+  <si>
+    <t>Alpha parameter for L-W</t>
+  </si>
+  <si>
+    <t>Beta parameter for L-W</t>
+  </si>
+  <si>
+    <t>equal size</t>
+  </si>
+  <si>
+    <t>equal distribution</t>
+  </si>
+  <si>
+    <t>fully mixed</t>
+  </si>
+  <si>
+    <t>Current Year</t>
+  </si>
+  <si>
+    <t>current year</t>
+  </si>
+  <si>
+    <t>`format(Sys.Date(), '%Y'))`</t>
   </si>
 </sst>
 </file>
@@ -1978,7 +2011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1991,6 +2024,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2271,24 +2308,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2310,8 +2349,14 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -2330,7 +2375,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -2349,7 +2394,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2368,7 +2413,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2389,7 +2434,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -2409,8 +2454,11 @@
       <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2431,7 +2479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -2451,8 +2499,11 @@
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="H8" s="8">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -2473,7 +2524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2493,8 +2544,14 @@
       <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -2515,7 +2572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -2535,8 +2592,11 @@
       <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -2557,7 +2617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -2577,8 +2637,11 @@
       <c r="G14" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="9">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -2599,7 +2662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -2619,8 +2682,11 @@
       <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H16" s="9">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -2641,7 +2707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -2661,8 +2727,11 @@
       <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -2683,7 +2752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -2704,7 +2773,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -2725,7 +2794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>48</v>
       </c>
@@ -2742,11 +2811,14 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>636</v>
       </c>
       <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="H22" s="9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -2763,11 +2835,14 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>637</v>
       </c>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -2787,8 +2862,14 @@
       <c r="G24" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -2808,8 +2889,14 @@
       <c r="G25" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="H25">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -2829,8 +2916,14 @@
       <c r="G26" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H26">
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -2850,8 +2943,11 @@
       <c r="G27" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -2878,25 +2974,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.453125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="51.26953125" style="3"/>
+    <col min="1" max="1" width="8.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="51.26953125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2918,8 +3016,14 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -2936,7 +3040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
@@ -2956,7 +3060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>61</v>
       </c>
@@ -2973,10 +3077,16 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+        <v>641</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="232" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -2993,7 +3103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>63</v>
       </c>
@@ -3010,7 +3120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>64</v>
       </c>
@@ -3027,7 +3137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>65</v>
       </c>
@@ -3047,7 +3157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>66</v>
       </c>
@@ -3066,8 +3176,11 @@
       <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>67</v>
       </c>
@@ -3086,8 +3199,11 @@
       <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>68</v>
       </c>
@@ -3106,8 +3222,11 @@
       <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>69</v>
       </c>
@@ -3126,8 +3245,11 @@
       <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>70</v>
       </c>
@@ -3147,7 +3269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>71</v>
       </c>
@@ -3155,7 +3277,7 @@
         <v>72</v>
       </c>
       <c r="C14" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>561</v>
@@ -3164,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>73</v>
       </c>
@@ -3183,8 +3305,11 @@
       <c r="G15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -3203,8 +3328,11 @@
       <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>75</v>
       </c>
@@ -3223,8 +3351,11 @@
       <c r="G17" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>76</v>
       </c>
@@ -3243,8 +3374,11 @@
       <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>77</v>
       </c>
@@ -3263,8 +3397,11 @@
       <c r="G19" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>232</v>
       </c>
@@ -3283,8 +3420,11 @@
       <c r="G20" s="3" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>233</v>
       </c>
@@ -3306,10 +3446,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3320,7 +3460,7 @@
     <col min="7" max="7" width="22.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3342,8 +3482,10 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3357,7 +3499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>200</v>
       </c>
@@ -3371,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -3385,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>202</v>
       </c>
@@ -3402,7 +3544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>203</v>
       </c>
@@ -3419,7 +3561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>204</v>
       </c>
@@ -3436,7 +3578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3453,7 +3595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>206</v>
       </c>
@@ -3467,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>207</v>
       </c>
@@ -3481,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>208</v>
       </c>
@@ -3495,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>209</v>
       </c>
@@ -3512,7 +3654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>210</v>
       </c>
@@ -3526,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>211</v>
       </c>
@@ -3540,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>212</v>
       </c>
@@ -3554,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>213</v>
       </c>
@@ -3785,22 +3927,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="136.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39" customWidth="1"/>
+    <col min="6" max="6" width="7.90625" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3822,8 +3965,14 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -3840,7 +3989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>226</v>
       </c>
@@ -3859,8 +4008,11 @@
       <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>227</v>
       </c>
@@ -3879,8 +4031,11 @@
       <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>228</v>
       </c>
@@ -3899,8 +4054,11 @@
       <c r="G5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>229</v>
       </c>
@@ -3919,8 +4077,11 @@
       <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>230</v>
       </c>
@@ -3939,8 +4100,11 @@
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>231</v>
       </c>
@@ -3958,6 +4122,9 @@
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3967,10 +4134,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3981,7 +4148,7 @@
     <col min="4" max="4" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>509</v>
       </c>
@@ -3994,8 +4161,10 @@
       <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>439</v>
       </c>
@@ -4009,7 +4178,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -4023,7 +4192,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -4037,7 +4206,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -4051,7 +4220,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -4065,7 +4234,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -4079,7 +4248,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -4093,7 +4262,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>442</v>
       </c>
@@ -4107,7 +4276,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -4121,7 +4290,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -4135,7 +4304,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -4149,7 +4318,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -4163,7 +4332,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>122</v>
       </c>
@@ -4177,7 +4346,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -4191,7 +4360,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
add V_real and retA_real to cpars
</commit_message>
<xml_diff>
--- a/build_tools/Class_definitions/Class_definitions.xlsx
+++ b/build_tools/Class_definitions/Class_definitions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2390" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-2390" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="648">
   <si>
     <t>Slot</t>
   </si>
@@ -1962,6 +1962,18 @@
   </si>
   <si>
     <t>`format(Sys.Date(), '%Y')`</t>
+  </si>
+  <si>
+    <t>V_real</t>
+  </si>
+  <si>
+    <t>retA_real</t>
+  </si>
+  <si>
+    <t>retL_real</t>
+  </si>
+  <si>
+    <t>SLarray_real</t>
   </si>
 </sst>
 </file>
@@ -2976,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -4150,10 +4162,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4714,13 +4726,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>644</v>
       </c>
       <c r="B41" t="s">
-        <v>197</v>
+        <v>444</v>
       </c>
       <c r="C41" t="s">
-        <v>198</v>
+        <v>132</v>
       </c>
       <c r="D41" t="s">
         <v>126</v>
@@ -4728,13 +4740,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>455</v>
+        <v>645</v>
       </c>
       <c r="B42" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="C42" t="s">
-        <v>457</v>
+        <v>135</v>
       </c>
       <c r="D42" t="s">
         <v>126</v>
@@ -4742,13 +4754,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>458</v>
+        <v>646</v>
       </c>
       <c r="B43" t="s">
-        <v>459</v>
+        <v>134</v>
       </c>
       <c r="C43" t="s">
-        <v>460</v>
+        <v>137</v>
       </c>
       <c r="D43" t="s">
         <v>126</v>
@@ -4756,83 +4768,83 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>232</v>
+        <v>647</v>
       </c>
       <c r="B44" t="s">
-        <v>461</v>
+        <v>134</v>
       </c>
       <c r="C44" t="s">
-        <v>462</v>
+        <v>139</v>
       </c>
       <c r="D44" t="s">
         <v>126</v>
       </c>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" t="s">
+        <v>197</v>
+      </c>
+      <c r="C45" t="s">
+        <v>198</v>
+      </c>
+      <c r="D45" t="s">
+        <v>126</v>
+      </c>
+    </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>456</v>
       </c>
       <c r="C46" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>459</v>
       </c>
       <c r="C47" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>467</v>
+        <v>232</v>
       </c>
       <c r="B48" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C48" t="s">
-        <v>610</v>
+        <v>462</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>608</v>
-      </c>
-      <c r="B49" t="s">
-        <v>468</v>
-      </c>
-      <c r="C49" t="s">
-        <v>609</v>
-      </c>
-      <c r="D49" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D50" t="s">
         <v>141</v>
@@ -4840,13 +4852,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B51" t="s">
-        <v>468</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="D51" t="s">
         <v>141</v>
@@ -4854,13 +4866,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B52" t="s">
         <v>468</v>
       </c>
       <c r="C52" t="s">
-        <v>487</v>
+        <v>610</v>
       </c>
       <c r="D52" t="s">
         <v>141</v>
@@ -4868,13 +4880,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>473</v>
+        <v>608</v>
       </c>
       <c r="B53" t="s">
         <v>468</v>
       </c>
       <c r="C53" t="s">
-        <v>488</v>
+        <v>609</v>
       </c>
       <c r="D53" t="s">
         <v>141</v>
@@ -4882,13 +4894,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B54" t="s">
         <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="D54" t="s">
         <v>141</v>
@@ -4896,13 +4908,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>471</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>468</v>
       </c>
       <c r="C55" t="s">
-        <v>164</v>
+        <v>486</v>
       </c>
       <c r="D55" t="s">
         <v>141</v>
@@ -4910,13 +4922,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B56" t="s">
         <v>468</v>
       </c>
       <c r="C56" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D56" t="s">
         <v>141</v>
@@ -4924,13 +4936,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>473</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>468</v>
       </c>
       <c r="C57" t="s">
-        <v>144</v>
+        <v>488</v>
       </c>
       <c r="D57" t="s">
         <v>141</v>
@@ -4938,13 +4950,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>474</v>
       </c>
       <c r="B58" t="s">
         <v>16</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>489</v>
       </c>
       <c r="D58" t="s">
         <v>141</v>
@@ -4952,13 +4964,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
         <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D59" t="s">
         <v>141</v>
@@ -4966,13 +4978,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>140</v>
+        <v>475</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>468</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>490</v>
       </c>
       <c r="D60" t="s">
         <v>141</v>
@@ -4980,13 +4992,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B61" t="s">
         <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D61" t="s">
         <v>141</v>
@@ -4994,13 +5006,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>476</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
         <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>485</v>
+        <v>154</v>
       </c>
       <c r="D62" t="s">
         <v>141</v>
@@ -5008,13 +5020,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>477</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
         <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>491</v>
+        <v>156</v>
       </c>
       <c r="D63" t="s">
         <v>141</v>
@@ -5022,13 +5034,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>478</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
         <v>16</v>
       </c>
       <c r="C64" t="s">
-        <v>492</v>
+        <v>142</v>
       </c>
       <c r="D64" t="s">
         <v>141</v>
@@ -5036,13 +5048,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>479</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
-        <v>468</v>
+        <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>493</v>
+        <v>152</v>
       </c>
       <c r="D65" t="s">
         <v>141</v>
@@ -5050,13 +5062,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>476</v>
       </c>
       <c r="B66" t="s">
         <v>16</v>
       </c>
       <c r="C66" t="s">
-        <v>146</v>
+        <v>485</v>
       </c>
       <c r="D66" t="s">
         <v>141</v>
@@ -5064,13 +5076,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>147</v>
+        <v>477</v>
       </c>
       <c r="B67" t="s">
         <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>148</v>
+        <v>491</v>
       </c>
       <c r="D67" t="s">
         <v>141</v>
@@ -5078,13 +5090,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>149</v>
+        <v>478</v>
       </c>
       <c r="B68" t="s">
         <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>492</v>
       </c>
       <c r="D68" t="s">
         <v>141</v>
@@ -5092,13 +5104,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>157</v>
+        <v>479</v>
       </c>
       <c r="B69" t="s">
-        <v>16</v>
+        <v>468</v>
       </c>
       <c r="C69" t="s">
-        <v>158</v>
+        <v>493</v>
       </c>
       <c r="D69" t="s">
         <v>141</v>
@@ -5106,13 +5118,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
         <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="D70" t="s">
         <v>141</v>
@@ -5120,13 +5132,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
         <v>16</v>
       </c>
       <c r="C71" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D71" t="s">
         <v>141</v>
@@ -5134,13 +5146,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>480</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
         <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>494</v>
+        <v>150</v>
       </c>
       <c r="D72" t="s">
         <v>141</v>
@@ -5148,13 +5160,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>481</v>
+        <v>157</v>
       </c>
       <c r="B73" t="s">
-        <v>468</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>495</v>
+        <v>158</v>
       </c>
       <c r="D73" t="s">
         <v>141</v>
@@ -5162,13 +5174,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>482</v>
+        <v>161</v>
       </c>
       <c r="B74" t="s">
         <v>16</v>
       </c>
       <c r="C74" t="s">
-        <v>496</v>
+        <v>162</v>
       </c>
       <c r="D74" t="s">
         <v>141</v>
@@ -5176,13 +5188,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>483</v>
+        <v>159</v>
       </c>
       <c r="B75" t="s">
-        <v>468</v>
+        <v>16</v>
       </c>
       <c r="C75" t="s">
-        <v>497</v>
+        <v>160</v>
       </c>
       <c r="D75" t="s">
         <v>141</v>
@@ -5190,13 +5202,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B76" t="s">
-        <v>468</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D76" t="s">
         <v>141</v>
@@ -5204,13 +5216,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>185</v>
+        <v>481</v>
       </c>
       <c r="B77" t="s">
-        <v>186</v>
+        <v>468</v>
       </c>
       <c r="C77" t="s">
-        <v>187</v>
+        <v>495</v>
       </c>
       <c r="D77" t="s">
         <v>141</v>
@@ -5218,13 +5230,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>188</v>
+        <v>482</v>
       </c>
       <c r="B78" t="s">
-        <v>189</v>
+        <v>16</v>
       </c>
       <c r="C78" t="s">
-        <v>190</v>
+        <v>496</v>
       </c>
       <c r="D78" t="s">
         <v>141</v>
@@ -5232,13 +5244,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>483</v>
       </c>
       <c r="B79" t="s">
-        <v>192</v>
+        <v>468</v>
       </c>
       <c r="C79" t="s">
-        <v>193</v>
+        <v>497</v>
       </c>
       <c r="D79" t="s">
         <v>141</v>
@@ -5246,13 +5258,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>165</v>
+        <v>484</v>
       </c>
       <c r="B80" t="s">
-        <v>16</v>
+        <v>468</v>
       </c>
       <c r="C80" t="s">
-        <v>166</v>
+        <v>498</v>
       </c>
       <c r="D80" t="s">
         <v>141</v>
@@ -5260,13 +5272,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>523</v>
+        <v>185</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="C81" t="s">
-        <v>526</v>
+        <v>187</v>
       </c>
       <c r="D81" t="s">
         <v>141</v>
@@ -5274,13 +5286,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>524</v>
+        <v>188</v>
       </c>
       <c r="B82" t="s">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="C82" t="s">
-        <v>527</v>
+        <v>190</v>
       </c>
       <c r="D82" t="s">
         <v>141</v>
@@ -5288,125 +5300,125 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>525</v>
+        <v>191</v>
       </c>
       <c r="B83" t="s">
-        <v>16</v>
+        <v>192</v>
       </c>
       <c r="C83" t="s">
-        <v>528</v>
+        <v>193</v>
       </c>
       <c r="D83" t="s">
         <v>141</v>
       </c>
     </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" t="s">
+        <v>166</v>
+      </c>
+      <c r="D84" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>611</v>
+        <v>523</v>
       </c>
       <c r="B85" t="s">
-        <v>625</v>
+        <v>16</v>
       </c>
       <c r="C85" t="s">
-        <v>614</v>
+        <v>526</v>
       </c>
       <c r="D85" t="s">
-        <v>617</v>
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>612</v>
+        <v>524</v>
       </c>
       <c r="B86" t="s">
-        <v>625</v>
+        <v>16</v>
       </c>
       <c r="C86" t="s">
-        <v>615</v>
+        <v>527</v>
       </c>
       <c r="D86" t="s">
-        <v>617</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>613</v>
+        <v>525</v>
       </c>
       <c r="B87" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" t="s">
+        <v>528</v>
+      </c>
+      <c r="D87" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>611</v>
+      </c>
+      <c r="B89" t="s">
         <v>625</v>
       </c>
-      <c r="C87" t="s">
-        <v>616</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C89" t="s">
+        <v>614</v>
+      </c>
+      <c r="D89" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>172</v>
+        <v>612</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>625</v>
       </c>
       <c r="C90" t="s">
-        <v>174</v>
+        <v>615</v>
       </c>
       <c r="D90" t="s">
-        <v>173</v>
+        <v>617</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>613</v>
       </c>
       <c r="B91" t="s">
-        <v>16</v>
+        <v>625</v>
       </c>
       <c r="C91" t="s">
-        <v>176</v>
+        <v>616</v>
       </c>
       <c r="D91" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>177</v>
-      </c>
-      <c r="B92" t="s">
-        <v>16</v>
-      </c>
-      <c r="C92" t="s">
-        <v>178</v>
-      </c>
-      <c r="D92" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>179</v>
-      </c>
-      <c r="B93" t="s">
-        <v>16</v>
-      </c>
-      <c r="C93" t="s">
-        <v>180</v>
-      </c>
-      <c r="D93" t="s">
-        <v>173</v>
+        <v>617</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B94" t="s">
         <v>16</v>
       </c>
       <c r="C94" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D94" t="s">
         <v>173</v>
@@ -5414,29 +5426,85 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B95" t="s">
         <v>16</v>
       </c>
       <c r="C95" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D95" t="s">
         <v>173</v>
       </c>
     </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>177</v>
+      </c>
+      <c r="B96" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" t="s">
+        <v>178</v>
+      </c>
+      <c r="D96" t="s">
+        <v>173</v>
+      </c>
+    </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>179</v>
+      </c>
+      <c r="B97" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" t="s">
+        <v>180</v>
+      </c>
+      <c r="D97" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>181</v>
+      </c>
+      <c r="B98" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" t="s">
+        <v>182</v>
+      </c>
+      <c r="D98" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>183</v>
+      </c>
+      <c r="B99" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" t="s">
+        <v>184</v>
+      </c>
+      <c r="D99" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>169</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B101" t="s">
         <v>170</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C101" t="s">
         <v>171</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D101" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add retA_real to cpars
</commit_message>
<xml_diff>
--- a/build_tools/Class_definitions/Class_definitions.xlsx
+++ b/build_tools/Class_definitions/Class_definitions.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="660">
   <si>
     <t>Slot</t>
   </si>
@@ -1974,6 +1974,42 @@
   </si>
   <si>
     <t>SLarray_real</t>
+  </si>
+  <si>
+    <t>L5_y</t>
+  </si>
+  <si>
+    <t>LFS_y</t>
+  </si>
+  <si>
+    <t>Vmaxlen_y</t>
+  </si>
+  <si>
+    <t>LR5_y</t>
+  </si>
+  <si>
+    <t>LFR_y</t>
+  </si>
+  <si>
+    <t>Rmaxlen_y</t>
+  </si>
+  <si>
+    <t>length-at-5 percent selection by sim and year</t>
+  </si>
+  <si>
+    <t>length at full selection by sim and year</t>
+  </si>
+  <si>
+    <t>vulnerability at max length by sim and year</t>
+  </si>
+  <si>
+    <t>length-at-5 percent retention by sim and year</t>
+  </si>
+  <si>
+    <t>length at full retention by sim and year</t>
+  </si>
+  <si>
+    <t>retention at max length by sim and year</t>
   </si>
 </sst>
 </file>
@@ -4162,10 +4198,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5506,6 +5542,90 @@
       </c>
       <c r="D101" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>648</v>
+      </c>
+      <c r="B103" t="s">
+        <v>468</v>
+      </c>
+      <c r="C103" t="s">
+        <v>654</v>
+      </c>
+      <c r="D103" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>649</v>
+      </c>
+      <c r="B104" t="s">
+        <v>468</v>
+      </c>
+      <c r="C104" t="s">
+        <v>655</v>
+      </c>
+      <c r="D104" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>650</v>
+      </c>
+      <c r="B105" t="s">
+        <v>468</v>
+      </c>
+      <c r="C105" t="s">
+        <v>656</v>
+      </c>
+      <c r="D105" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>651</v>
+      </c>
+      <c r="B106" t="s">
+        <v>468</v>
+      </c>
+      <c r="C106" t="s">
+        <v>657</v>
+      </c>
+      <c r="D106" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>652</v>
+      </c>
+      <c r="B107" t="s">
+        <v>468</v>
+      </c>
+      <c r="C107" t="s">
+        <v>658</v>
+      </c>
+      <c r="D107" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>653</v>
+      </c>
+      <c r="B108" t="s">
+        <v>468</v>
+      </c>
+      <c r="C108" t="s">
+        <v>659</v>
+      </c>
+      <c r="D108" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Real.Data.Map to cpars
</commit_message>
<xml_diff>
--- a/build_tools/Class_definitions/Class_definitions.xlsx
+++ b/build_tools/Class_definitions/Class_definitions.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="663">
   <si>
     <t>Slot</t>
   </si>
@@ -2010,6 +2010,15 @@
   </si>
   <si>
     <t>retention at max length by sim and year</t>
+  </si>
+  <si>
+    <t>Real.Data.Map</t>
+  </si>
+  <si>
+    <t>numeric matrix dim=c(n.fleet, n.stock)</t>
+  </si>
+  <si>
+    <t>Map real data across stocks</t>
   </si>
 </sst>
 </file>
@@ -4198,15 +4207,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.453125" customWidth="1"/>
@@ -5626,6 +5635,20 @@
       </c>
       <c r="D108" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>660</v>
+      </c>
+      <c r="B110" t="s">
+        <v>661</v>
+      </c>
+      <c r="C110" t="s">
+        <v>662</v>
+      </c>
+      <c r="D110" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>